<commit_message>
Wk6 analysis and bug fixes
</commit_message>
<xml_diff>
--- a/scrapePage/schedule_2023_06.xlsx
+++ b/scrapePage/schedule_2023_06.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\program_project\CFB\scrapePage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D5567082-4566-4D0A-AA49-5DB752428B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116739A7-F393-4F72-9BE8-55BD1FBEE0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule_2023_06" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -298,7 +311,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,11 +449,11 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF2B2C2D"/>
+      <color rgb="FFFF0000"/>
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -629,6 +642,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,11 +812,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1152,11 +1172,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,18 +1198,18 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1205,7 +1225,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1232,7 +1252,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1259,40 +1279,40 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1308,13 +1328,13 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1407,24 +1427,24 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1528,13 +1548,13 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1605,13 +1625,13 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1638,35 +1658,35 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1693,13 +1713,13 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1748,17 +1768,18 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>